<commit_message>
Editing SPMP to reflect new updates to gantt/deliverables
</commit_message>
<xml_diff>
--- a/repo docs/groupgantt.xlsx
+++ b/repo docs/groupgantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seanh\Desktop\COSC 412\groupmaster412\COSC-412-Group-Project\repo docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F22CC4-3EAE-4993-917B-6579E8EEC1D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B3A855-595A-46B7-B3A4-EA8D2D4E607C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1144,8 +1144,8 @@
   </sheetPr>
   <dimension ref="B1:BO37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1742,7 +1742,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="8">
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updating requirements to reflect use cases
</commit_message>
<xml_diff>
--- a/repo docs/groupgantt.xlsx
+++ b/repo docs/groupgantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seanh\Desktop\COSC 412\groupmaster412\COSC-412-Group-Project\repo docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B3A855-595A-46B7-B3A4-EA8D2D4E607C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD378C12-0D2C-4C04-954A-67DE0E4E0191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -241,7 +241,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -352,6 +352,20 @@
       <b/>
       <sz val="13"/>
       <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -594,7 +608,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -732,6 +746,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1144,8 +1167,8 @@
   </sheetPr>
   <dimension ref="B1:BO37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1485,7 +1508,7 @@
       </c>
     </row>
     <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="46" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="25">
@@ -1505,7 +1528,7 @@
       </c>
     </row>
     <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="47" t="s">
         <v>34</v>
       </c>
       <c r="C6" s="7">
@@ -1525,7 +1548,7 @@
       </c>
     </row>
     <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="46" t="s">
         <v>38</v>
       </c>
       <c r="C7" s="25">
@@ -1545,7 +1568,7 @@
       </c>
     </row>
     <row r="8" spans="2:67" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="47" t="s">
         <v>25</v>
       </c>
       <c r="C8" s="7">
@@ -1565,7 +1588,7 @@
       </c>
     </row>
     <row r="9" spans="2:67" ht="54" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="46" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="25">
@@ -1588,7 +1611,7 @@
       </c>
     </row>
     <row r="10" spans="2:67" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="47" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="7">
@@ -1608,7 +1631,7 @@
       </c>
     </row>
     <row r="11" spans="2:67" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="47" t="s">
         <v>41</v>
       </c>
       <c r="C11" s="7">
@@ -1623,10 +1646,12 @@
       <c r="F11" s="7">
         <v>1</v>
       </c>
-      <c r="G11" s="8"/>
+      <c r="G11" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="2:67" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="46" t="s">
         <v>27</v>
       </c>
       <c r="C12" s="25">
@@ -1646,7 +1671,7 @@
       </c>
     </row>
     <row r="13" spans="2:67" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="47" t="s">
         <v>37</v>
       </c>
       <c r="C13" s="7">
@@ -1662,11 +1687,11 @@
         <v>1</v>
       </c>
       <c r="G13" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:67" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="46" t="s">
         <v>31</v>
       </c>
       <c r="C14" s="25">
@@ -1682,11 +1707,11 @@
         <v>1</v>
       </c>
       <c r="G14" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:67" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="48" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="7">
@@ -1706,7 +1731,7 @@
       </c>
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="46" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="28">
@@ -1726,7 +1751,7 @@
       </c>
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="48" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="7">
@@ -1746,7 +1771,7 @@
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="46" t="s">
         <v>35</v>
       </c>
       <c r="C18" s="25">
@@ -1766,7 +1791,7 @@
       </c>
     </row>
     <row r="19" spans="2:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="47" t="s">
         <v>24</v>
       </c>
       <c r="C19" s="7">
@@ -1786,7 +1811,7 @@
       </c>
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="46" t="s">
         <v>28</v>
       </c>
       <c r="C20" s="25">

</xml_diff>

<commit_message>
updated SPMP and gantt chart
</commit_message>
<xml_diff>
--- a/repo docs/groupgantt.xlsx
+++ b/repo docs/groupgantt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seanh\Desktop\COSC 412\groupmaster412\COSC-412-Group-Project\repo docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Downloads\School\Git\repo docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD378C12-0D2C-4C04-954A-67DE0E4E0191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E58DF68-DBB9-4871-95E0-8261FE5BE84D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -699,6 +699,15 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -746,15 +755,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1167,8 +1167,8 @@
   </sheetPr>
   <dimension ref="B1:BO37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="U12" sqref="U12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1220,13 +1220,13 @@
       </c>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
       <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1234,66 +1234,66 @@
         <v>32</v>
       </c>
       <c r="J2" s="20"/>
-      <c r="K2" s="38" t="s">
+      <c r="K2" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="40"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="43"/>
       <c r="P2" s="14"/>
-      <c r="Q2" s="38" t="s">
+      <c r="Q2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="41"/>
-      <c r="S2" s="41"/>
-      <c r="T2" s="40"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="43"/>
       <c r="U2" s="15"/>
-      <c r="V2" s="30" t="s">
+      <c r="V2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="42"/>
+      <c r="W2" s="34"/>
+      <c r="X2" s="34"/>
+      <c r="Y2" s="45"/>
       <c r="Z2" s="16"/>
-      <c r="AA2" s="43" t="s">
+      <c r="AA2" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="AB2" s="44"/>
-      <c r="AC2" s="44"/>
-      <c r="AD2" s="44"/>
-      <c r="AE2" s="44"/>
-      <c r="AF2" s="44"/>
-      <c r="AG2" s="45"/>
+      <c r="AB2" s="47"/>
+      <c r="AC2" s="47"/>
+      <c r="AD2" s="47"/>
+      <c r="AE2" s="47"/>
+      <c r="AF2" s="47"/>
+      <c r="AG2" s="48"/>
       <c r="AH2" s="17"/>
-      <c r="AI2" s="30" t="s">
+      <c r="AI2" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="AJ2" s="31"/>
-      <c r="AK2" s="31"/>
-      <c r="AL2" s="31"/>
-      <c r="AM2" s="31"/>
-      <c r="AN2" s="31"/>
-      <c r="AO2" s="31"/>
-      <c r="AP2" s="31"/>
+      <c r="AJ2" s="34"/>
+      <c r="AK2" s="34"/>
+      <c r="AL2" s="34"/>
+      <c r="AM2" s="34"/>
+      <c r="AN2" s="34"/>
+      <c r="AO2" s="34"/>
+      <c r="AP2" s="34"/>
     </row>
     <row r="3" spans="2:67" s="11" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="35" t="s">
+      <c r="B3" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="37" t="s">
+      <c r="G3" s="40" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="18" t="s">
@@ -1320,12 +1320,12 @@
       <c r="AA3" s="10"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="34"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1508,7 +1508,7 @@
       </c>
     </row>
     <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="30" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="25">
@@ -1528,7 +1528,7 @@
       </c>
     </row>
     <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="31" t="s">
         <v>34</v>
       </c>
       <c r="C6" s="7">
@@ -1548,7 +1548,7 @@
       </c>
     </row>
     <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="30" t="s">
         <v>38</v>
       </c>
       <c r="C7" s="25">
@@ -1568,7 +1568,7 @@
       </c>
     </row>
     <row r="8" spans="2:67" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="31" t="s">
         <v>25</v>
       </c>
       <c r="C8" s="7">
@@ -1588,7 +1588,7 @@
       </c>
     </row>
     <row r="9" spans="2:67" ht="54" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="30" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="25">
@@ -1611,7 +1611,7 @@
       </c>
     </row>
     <row r="10" spans="2:67" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="31" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="7">
@@ -1631,7 +1631,7 @@
       </c>
     </row>
     <row r="11" spans="2:67" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="31" t="s">
         <v>41</v>
       </c>
       <c r="C11" s="7">
@@ -1651,7 +1651,7 @@
       </c>
     </row>
     <row r="12" spans="2:67" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="30" t="s">
         <v>27</v>
       </c>
       <c r="C12" s="25">
@@ -1671,7 +1671,7 @@
       </c>
     </row>
     <row r="13" spans="2:67" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="31" t="s">
         <v>37</v>
       </c>
       <c r="C13" s="7">
@@ -1691,7 +1691,7 @@
       </c>
     </row>
     <row r="14" spans="2:67" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="30" t="s">
         <v>31</v>
       </c>
       <c r="C14" s="25">
@@ -1711,7 +1711,7 @@
       </c>
     </row>
     <row r="15" spans="2:67" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="32" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="7">
@@ -1731,7 +1731,7 @@
       </c>
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="30" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="28">
@@ -1751,7 +1751,7 @@
       </c>
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="32" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="7">
@@ -1771,7 +1771,7 @@
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="30" t="s">
         <v>35</v>
       </c>
       <c r="C18" s="25">
@@ -1787,11 +1787,11 @@
         <v>2</v>
       </c>
       <c r="G18" s="26">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="31" t="s">
         <v>24</v>
       </c>
       <c r="C19" s="7">
@@ -1811,7 +1811,7 @@
       </c>
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="46" t="s">
+      <c r="B20" s="30" t="s">
         <v>28</v>
       </c>
       <c r="C20" s="25">
@@ -1827,7 +1827,7 @@
         <v>2</v>
       </c>
       <c r="G20" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update group gantt chart
Gantt Chart update after meeting with group
</commit_message>
<xml_diff>
--- a/repo docs/groupgantt.xlsx
+++ b/repo docs/groupgantt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Downloads\School\Git\repo docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seanh\Desktop\COSC 412\groupmaster412\COSC-412-Group-Project\repo docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E58DF68-DBB9-4871-95E0-8261FE5BE84D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5501A6-1A4B-4BDE-97E7-BA29E2722543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -1167,8 +1167,8 @@
   </sheetPr>
   <dimension ref="B1:BO37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1647,7 +1647,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="8">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="12" spans="2:67" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1727,7 +1727,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1747,7 +1747,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1767,7 +1767,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="8">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1787,7 +1787,7 @@
         <v>2</v>
       </c>
       <c r="G18" s="26">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1807,7 +1807,7 @@
         <v>3</v>
       </c>
       <c r="G19" s="8">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1867,7 +1867,7 @@
         <v>2</v>
       </c>
       <c r="G22" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>